<commit_message>
Added working TSS and GreedyTSS
</commit_message>
<xml_diff>
--- a/Results/Greedy.xlsx
+++ b/Results/Greedy.xlsx
@@ -361,7 +361,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +395,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">

</xml_diff>

<commit_message>
New results to greedy and added some changes based off advises
</commit_message>
<xml_diff>
--- a/Results/Greedy.xlsx
+++ b/Results/Greedy.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Blog Catalog 3</t>
+  </si>
+  <si>
+    <t>Douban</t>
   </si>
 </sst>
 </file>
@@ -358,85 +361,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>91</v>
+      </c>
+      <c r="C11">
+        <v>3998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>